<commit_message>
major major major improvements
</commit_message>
<xml_diff>
--- a/inst/extdata/james-example-one-tab.xlsx
+++ b/inst/extdata/james-example-one-tab.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdijkstra/Dropbox/cpb/git/james-package/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEAFF15F-959F-1247-829F-7EF60B2769E3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0453A446-AC92-944E-9DA8-F6DE2ADF07C8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="3060" windowWidth="28040" windowHeight="17440" xr2:uid="{9E6F58C3-28B5-A945-A3C1-97A0DEA814F4}"/>
   </bookViews>
@@ -25,12 +25,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>bbp</t>
+    <t/>
   </si>
   <si>
-    <t>happiness</t>
+    <t>consumptie huishoudens</t>
+  </si>
+  <si>
+    <t>investeringen in woningen</t>
+  </si>
+  <si>
+    <t>bedrijfsinvesteringen</t>
+  </si>
+  <si>
+    <t>overheidsbestedingen</t>
+  </si>
+  <si>
+    <t>uitvoer</t>
+  </si>
+  <si>
+    <t>bbp-groei</t>
   </si>
 </sst>
 </file>
@@ -66,8 +81,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,97 +398,205 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BD9CBB1-A8EF-C741-8579-6592F6909FA2}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.83203125" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2000</v>
-      </c>
-      <c r="B2">
-        <v>500</v>
-      </c>
-      <c r="C2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2013</v>
+      </c>
+      <c r="B2" s="1">
+        <v>-0.49686056056014999</v>
+      </c>
+      <c r="C2" s="1">
+        <v>-0.37524195707708302</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.150499337528466</v>
+      </c>
+      <c r="E2" s="1">
+        <v>-0.12649590593452301</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.71792815077837002</v>
+      </c>
+      <c r="G2" s="1">
+        <v>-0.124857872221618</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2001</v>
-      </c>
-      <c r="B3">
-        <v>500</v>
-      </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2014</v>
+      </c>
+      <c r="B3" s="1">
+        <v>8.2888168875883905E-2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.202460452469683</v>
+      </c>
+      <c r="D3" s="1">
+        <v>-7.2549583537743906E-2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>4.2448300865373503E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1.16816001528366</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1.42379459921866</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2002</v>
-      </c>
-      <c r="B4">
-        <v>1000</v>
-      </c>
-      <c r="C4">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2015</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.30718553055271802</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.45544637757114897</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.51660946251314199</v>
+      </c>
+      <c r="E4" s="1">
+        <v>-6.7094840138109804E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.74729925769011396</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1.96066341486858</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>2003</v>
-      </c>
-      <c r="B5">
-        <v>500</v>
-      </c>
-      <c r="C5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2016</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.35769030558478099</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.60386539481202595</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.42815893114750597</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.26491741429794902</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.53731049316076895</v>
+      </c>
+      <c r="G5" s="1">
+        <v>2.1898772987727799</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2004</v>
-      </c>
-      <c r="B6">
-        <v>500</v>
-      </c>
-      <c r="C6">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2017</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.57409637317529605</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.371589605181181</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.25467584592030101</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.320894761656915</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1.34772092959482</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2.86674805827385</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2005</v>
-      </c>
-      <c r="B7">
-        <v>500</v>
-      </c>
-      <c r="C7">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2018</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2.77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>2006</v>
-      </c>
-      <c r="B8">
-        <v>500</v>
-      </c>
-      <c r="C8">
-        <v>98</v>
+        <v>2019</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="G8" s="1">
+        <v>2.57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>